<commit_message>
finished refactoring for python package #20
successfully completed the transition from a single imported python file to a local python package

note: pyscript appears not to be able to access sys module
</commit_message>
<xml_diff>
--- a/main/database/yandiya-db.xlsx
+++ b/main/database/yandiya-db.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -394,42 +394,33 @@
         <v>productTitle</v>
       </c>
       <c r="E1" t="str">
-        <v>pWidth</v>
+        <v>icWidth</v>
       </c>
       <c r="F1" t="str">
-        <v>pHeight</v>
+        <v>icHeight</v>
       </c>
       <c r="G1" t="str">
-        <v>pDepth</v>
+        <v>icDepth</v>
       </c>
       <c r="H1" t="str">
-        <v>icWidth</v>
+        <v>icWeight</v>
       </c>
       <c r="I1" t="str">
-        <v>icHeight</v>
+        <v>icQty</v>
       </c>
       <c r="J1" t="str">
-        <v>icDepth</v>
+        <v>ocWidth</v>
       </c>
       <c r="K1" t="str">
-        <v>icWeight</v>
+        <v>ocHeight</v>
       </c>
       <c r="L1" t="str">
-        <v>icQty</v>
+        <v>ocDepth</v>
       </c>
       <c r="M1" t="str">
-        <v>ocWidth</v>
+        <v>ocWeight</v>
       </c>
       <c r="N1" t="str">
-        <v>ocHeight</v>
-      </c>
-      <c r="O1" t="str">
-        <v>ocDepth</v>
-      </c>
-      <c r="P1" t="str">
-        <v>ocWeight</v>
-      </c>
-      <c r="Q1" t="str">
         <v>ocQty</v>
       </c>
     </row>
@@ -447,42 +438,33 @@
         <v>Aluminium Panel Heater W (350W)</v>
       </c>
       <c r="E2" t="str">
-        <v>595</v>
+        <v>670</v>
       </c>
       <c r="F2" t="str">
-        <v>595</v>
+        <v>660</v>
       </c>
       <c r="G2" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H2" t="str">
-        <v>670</v>
+        <v>4.78</v>
       </c>
       <c r="I2" t="str">
-        <v>660</v>
+        <v>1</v>
       </c>
       <c r="J2" t="str">
-        <v>50</v>
+        <v>700</v>
       </c>
       <c r="K2" t="str">
-        <v>4.78</v>
+        <v>710</v>
       </c>
       <c r="L2" t="str">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="M2" t="str">
-        <v>700</v>
+        <v>25.92</v>
       </c>
       <c r="N2" t="str">
-        <v>710</v>
-      </c>
-      <c r="O2" t="str">
-        <v>250</v>
-      </c>
-      <c r="P2" t="str">
-        <v>25.92</v>
-      </c>
-      <c r="Q2" t="str">
         <v>5</v>
       </c>
     </row>
@@ -500,42 +482,33 @@
         <v>Aluminium Panel Heater W (500W)</v>
       </c>
       <c r="E3" t="str">
-        <v>795</v>
+        <v>670</v>
       </c>
       <c r="F3" t="str">
-        <v>595</v>
+        <v>860</v>
       </c>
       <c r="G3" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H3" t="str">
-        <v>670</v>
+        <v>6.5</v>
       </c>
       <c r="I3" t="str">
-        <v>860</v>
+        <v>1</v>
       </c>
       <c r="J3" t="str">
-        <v>50</v>
+        <v>705</v>
       </c>
       <c r="K3" t="str">
-        <v>6.5</v>
+        <v>870</v>
       </c>
       <c r="L3" t="str">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="M3" t="str">
-        <v>705</v>
+        <v>35.33</v>
       </c>
       <c r="N3" t="str">
-        <v>870</v>
-      </c>
-      <c r="O3" t="str">
-        <v>265</v>
-      </c>
-      <c r="P3" t="str">
-        <v>35.33</v>
-      </c>
-      <c r="Q3" t="str">
         <v>5</v>
       </c>
     </row>
@@ -553,42 +526,33 @@
         <v>Aluminium Panel Heater W (800W)</v>
       </c>
       <c r="E4" t="str">
-        <v>1195</v>
+        <v>670</v>
       </c>
       <c r="F4" t="str">
-        <v>595</v>
+        <v>1267</v>
       </c>
       <c r="G4" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H4" t="str">
-        <v>670</v>
+        <v>10</v>
       </c>
       <c r="I4" t="str">
-        <v>1267</v>
+        <v>1</v>
       </c>
       <c r="J4" t="str">
-        <v>50</v>
+        <v>710</v>
       </c>
       <c r="K4" t="str">
-        <v>10</v>
+        <v>1305</v>
       </c>
       <c r="L4" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M4" t="str">
-        <v>710</v>
+        <v>54</v>
       </c>
       <c r="N4" t="str">
-        <v>1305</v>
-      </c>
-      <c r="O4" t="str">
-        <v>270</v>
-      </c>
-      <c r="P4" t="str">
-        <v>54</v>
-      </c>
-      <c r="Q4" t="str">
         <v>5</v>
       </c>
     </row>
@@ -606,42 +570,33 @@
         <v>Aluminium Panel Heater W (1200W)</v>
       </c>
       <c r="E5" t="str">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="F5" t="str">
-        <v>800</v>
+        <v>1253</v>
       </c>
       <c r="G5" t="str">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="H5" t="str">
+        <v>12.84</v>
+      </c>
+      <c r="I5" t="str">
+        <v>1</v>
+      </c>
+      <c r="J5" t="str">
         <v>870</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="str">
         <v>1253</v>
       </c>
-      <c r="J5" t="str">
+      <c r="L5" t="str">
         <v>55</v>
       </c>
-      <c r="K5" t="str">
-        <v>12.84</v>
-      </c>
-      <c r="L5" t="str">
-        <v>1</v>
-      </c>
       <c r="M5" t="str">
-        <v>870</v>
+        <v>13</v>
       </c>
       <c r="N5" t="str">
-        <v>1253</v>
-      </c>
-      <c r="O5" t="str">
-        <v>55</v>
-      </c>
-      <c r="P5" t="str">
-        <v>13</v>
-      </c>
-      <c r="Q5" t="str">
         <v>1</v>
       </c>
     </row>
@@ -659,42 +614,33 @@
         <v>Aluminium Panel Heater W (600W)</v>
       </c>
       <c r="E6" t="str">
-        <v>2000</v>
+        <v>385</v>
       </c>
       <c r="F6" t="str">
-        <v>250</v>
+        <v>2030</v>
       </c>
       <c r="G6" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H6" t="str">
-        <v>385</v>
+        <v>7.77</v>
       </c>
       <c r="I6" t="str">
-        <v>2030</v>
+        <v>1</v>
       </c>
       <c r="J6" t="str">
-        <v>50</v>
+        <v>680</v>
       </c>
       <c r="K6" t="str">
-        <v>7.77</v>
+        <v>2065</v>
       </c>
       <c r="L6" t="str">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="M6" t="str">
-        <v>680</v>
+        <v>16.54</v>
       </c>
       <c r="N6" t="str">
-        <v>2065</v>
-      </c>
-      <c r="O6" t="str">
-        <v>105</v>
-      </c>
-      <c r="P6" t="str">
-        <v>16.54</v>
-      </c>
-      <c r="Q6" t="str">
         <v>2</v>
       </c>
     </row>
@@ -712,42 +658,33 @@
         <v>Aluminium Panel Heater B (350W)</v>
       </c>
       <c r="E7" t="str">
-        <v>595</v>
+        <v>670</v>
       </c>
       <c r="F7" t="str">
-        <v>595</v>
+        <v>660</v>
       </c>
       <c r="G7" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H7" t="str">
-        <v>670</v>
+        <v>4.78</v>
       </c>
       <c r="I7" t="str">
-        <v>660</v>
+        <v>1</v>
       </c>
       <c r="J7" t="str">
-        <v>50</v>
+        <v>700</v>
       </c>
       <c r="K7" t="str">
-        <v>4.78</v>
+        <v>710</v>
       </c>
       <c r="L7" t="str">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="M7" t="str">
-        <v>700</v>
+        <v>25.92</v>
       </c>
       <c r="N7" t="str">
-        <v>710</v>
-      </c>
-      <c r="O7" t="str">
-        <v>250</v>
-      </c>
-      <c r="P7" t="str">
-        <v>25.92</v>
-      </c>
-      <c r="Q7" t="str">
         <v>5</v>
       </c>
     </row>
@@ -765,42 +702,33 @@
         <v>Aluminium Panel Heater B (500W)</v>
       </c>
       <c r="E8" t="str">
-        <v>795</v>
+        <v>670</v>
       </c>
       <c r="F8" t="str">
-        <v>595</v>
+        <v>860</v>
       </c>
       <c r="G8" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H8" t="str">
-        <v>670</v>
+        <v>6.5</v>
       </c>
       <c r="I8" t="str">
-        <v>860</v>
+        <v>1</v>
       </c>
       <c r="J8" t="str">
-        <v>50</v>
+        <v>705</v>
       </c>
       <c r="K8" t="str">
-        <v>6.5</v>
+        <v>870</v>
       </c>
       <c r="L8" t="str">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="M8" t="str">
-        <v>705</v>
+        <v>35.33</v>
       </c>
       <c r="N8" t="str">
-        <v>870</v>
-      </c>
-      <c r="O8" t="str">
-        <v>265</v>
-      </c>
-      <c r="P8" t="str">
-        <v>35.33</v>
-      </c>
-      <c r="Q8" t="str">
         <v>5</v>
       </c>
     </row>
@@ -818,42 +746,33 @@
         <v>Aluminium Panel Heater B (600W)</v>
       </c>
       <c r="E9" t="str">
-        <v>2000</v>
+        <v>385</v>
       </c>
       <c r="F9" t="str">
-        <v>250</v>
+        <v>2030</v>
       </c>
       <c r="G9" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H9" t="str">
-        <v>385</v>
+        <v>7.77</v>
       </c>
       <c r="I9" t="str">
-        <v>2030</v>
+        <v>1</v>
       </c>
       <c r="J9" t="str">
-        <v>50</v>
+        <v>680</v>
       </c>
       <c r="K9" t="str">
-        <v>7.77</v>
+        <v>2065</v>
       </c>
       <c r="L9" t="str">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="M9" t="str">
-        <v>680</v>
+        <v>16.54</v>
       </c>
       <c r="N9" t="str">
-        <v>2065</v>
-      </c>
-      <c r="O9" t="str">
-        <v>105</v>
-      </c>
-      <c r="P9" t="str">
-        <v>16.54</v>
-      </c>
-      <c r="Q9" t="str">
         <v>2</v>
       </c>
     </row>
@@ -871,42 +790,33 @@
         <v>Aluminium Panel Heater B (800W)</v>
       </c>
       <c r="E10" t="str">
-        <v>1195</v>
+        <v>670</v>
       </c>
       <c r="F10" t="str">
-        <v>595</v>
+        <v>1267</v>
       </c>
       <c r="G10" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H10" t="str">
-        <v>670</v>
+        <v>10</v>
       </c>
       <c r="I10" t="str">
-        <v>1267</v>
+        <v>1</v>
       </c>
       <c r="J10" t="str">
-        <v>50</v>
+        <v>710</v>
       </c>
       <c r="K10" t="str">
-        <v>10</v>
+        <v>1305</v>
       </c>
       <c r="L10" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M10" t="str">
-        <v>710</v>
+        <v>54</v>
       </c>
       <c r="N10" t="str">
-        <v>1305</v>
-      </c>
-      <c r="O10" t="str">
-        <v>270</v>
-      </c>
-      <c r="P10" t="str">
-        <v>54</v>
-      </c>
-      <c r="Q10" t="str">
         <v>5</v>
       </c>
     </row>
@@ -924,42 +834,33 @@
         <v>Aluminium Panel Heater B (1200W)</v>
       </c>
       <c r="E11" t="str">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="F11" t="str">
-        <v>800</v>
+        <v>1253</v>
       </c>
       <c r="G11" t="str">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="H11" t="str">
+        <v>12.84</v>
+      </c>
+      <c r="I11" t="str">
+        <v>1</v>
+      </c>
+      <c r="J11" t="str">
         <v>870</v>
       </c>
-      <c r="I11" t="str">
+      <c r="K11" t="str">
         <v>1253</v>
       </c>
-      <c r="J11" t="str">
+      <c r="L11" t="str">
         <v>55</v>
       </c>
-      <c r="K11" t="str">
-        <v>12.84</v>
-      </c>
-      <c r="L11" t="str">
-        <v>1</v>
-      </c>
       <c r="M11" t="str">
-        <v>870</v>
+        <v>13</v>
       </c>
       <c r="N11" t="str">
-        <v>1253</v>
-      </c>
-      <c r="O11" t="str">
-        <v>55</v>
-      </c>
-      <c r="P11" t="str">
-        <v>13</v>
-      </c>
-      <c r="Q11" t="str">
         <v>1</v>
       </c>
     </row>
@@ -977,42 +878,33 @@
         <v>Aluminium Panel Heater P (350W)</v>
       </c>
       <c r="E12" t="str">
-        <v>595</v>
+        <v>670</v>
       </c>
       <c r="F12" t="str">
-        <v>595</v>
+        <v>660</v>
       </c>
       <c r="G12" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H12" t="str">
-        <v>670</v>
+        <v>4.78</v>
       </c>
       <c r="I12" t="str">
-        <v>660</v>
+        <v>1</v>
       </c>
       <c r="J12" t="str">
-        <v>50</v>
+        <v>705</v>
       </c>
       <c r="K12" t="str">
-        <v>4.78</v>
+        <v>705</v>
       </c>
       <c r="L12" t="str">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="M12" t="str">
-        <v>705</v>
+        <v>25.92</v>
       </c>
       <c r="N12" t="str">
-        <v>705</v>
-      </c>
-      <c r="O12" t="str">
-        <v>250</v>
-      </c>
-      <c r="P12" t="str">
-        <v>25.92</v>
-      </c>
-      <c r="Q12" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1030,42 +922,33 @@
         <v>Aluminium Panel Heater P (500W)</v>
       </c>
       <c r="E13" t="str">
-        <v>795</v>
+        <v>670</v>
       </c>
       <c r="F13" t="str">
-        <v>595</v>
+        <v>860</v>
       </c>
       <c r="G13" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H13" t="str">
-        <v>670</v>
+        <v>6.5</v>
       </c>
       <c r="I13" t="str">
-        <v>860</v>
+        <v>1</v>
       </c>
       <c r="J13" t="str">
-        <v>50</v>
+        <v>705</v>
       </c>
       <c r="K13" t="str">
-        <v>6.5</v>
+        <v>870</v>
       </c>
       <c r="L13" t="str">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="M13" t="str">
-        <v>705</v>
+        <v>35.33</v>
       </c>
       <c r="N13" t="str">
-        <v>870</v>
-      </c>
-      <c r="O13" t="str">
-        <v>265</v>
-      </c>
-      <c r="P13" t="str">
-        <v>35.33</v>
-      </c>
-      <c r="Q13" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1083,42 +966,33 @@
         <v>Aluminium Panel Heater P (800W)</v>
       </c>
       <c r="E14" t="str">
-        <v>1195</v>
+        <v>670</v>
       </c>
       <c r="F14" t="str">
-        <v>595</v>
+        <v>1260</v>
       </c>
       <c r="G14" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H14" t="str">
-        <v>670</v>
+        <v>7.77</v>
       </c>
       <c r="I14" t="str">
-        <v>1260</v>
+        <v>1</v>
       </c>
       <c r="J14" t="str">
-        <v>50</v>
+        <v>710</v>
       </c>
       <c r="K14" t="str">
-        <v>7.77</v>
+        <v>1305</v>
       </c>
       <c r="L14" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M14" t="str">
-        <v>710</v>
+        <v>16.54</v>
       </c>
       <c r="N14" t="str">
-        <v>1305</v>
-      </c>
-      <c r="O14" t="str">
-        <v>270</v>
-      </c>
-      <c r="P14" t="str">
-        <v>16.54</v>
-      </c>
-      <c r="Q14" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1136,42 +1010,33 @@
         <v>Aluminium Panel Heater LST-W (350W)</v>
       </c>
       <c r="E15" t="str">
-        <v>595</v>
+        <v>670</v>
       </c>
       <c r="F15" t="str">
-        <v>595</v>
+        <v>660</v>
       </c>
       <c r="G15" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H15" t="str">
-        <v>670</v>
+        <v>4.78</v>
       </c>
       <c r="I15" t="str">
-        <v>660</v>
+        <v>1</v>
       </c>
       <c r="J15" t="str">
-        <v>50</v>
+        <v>705</v>
       </c>
       <c r="K15" t="str">
-        <v>4.78</v>
+        <v>705</v>
       </c>
       <c r="L15" t="str">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="M15" t="str">
-        <v>705</v>
+        <v>25.92</v>
       </c>
       <c r="N15" t="str">
-        <v>705</v>
-      </c>
-      <c r="O15" t="str">
-        <v>250</v>
-      </c>
-      <c r="P15" t="str">
-        <v>25.92</v>
-      </c>
-      <c r="Q15" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1189,42 +1054,33 @@
         <v>Aluminium Panel Heater LST-W (500W)</v>
       </c>
       <c r="E16" t="str">
-        <v>795</v>
+        <v>670</v>
       </c>
       <c r="F16" t="str">
-        <v>595</v>
+        <v>860</v>
       </c>
       <c r="G16" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H16" t="str">
-        <v>670</v>
+        <v>6.5</v>
       </c>
       <c r="I16" t="str">
-        <v>860</v>
+        <v>1</v>
       </c>
       <c r="J16" t="str">
-        <v>50</v>
+        <v>705</v>
       </c>
       <c r="K16" t="str">
-        <v>6.5</v>
+        <v>870</v>
       </c>
       <c r="L16" t="str">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="M16" t="str">
-        <v>705</v>
+        <v>35.33</v>
       </c>
       <c r="N16" t="str">
-        <v>870</v>
-      </c>
-      <c r="O16" t="str">
-        <v>265</v>
-      </c>
-      <c r="P16" t="str">
-        <v>35.33</v>
-      </c>
-      <c r="Q16" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1242,42 +1098,33 @@
         <v>Aluminium Panel Heater LST-W (800W)</v>
       </c>
       <c r="E17" t="str">
-        <v>1195</v>
+        <v>670</v>
       </c>
       <c r="F17" t="str">
-        <v>595</v>
+        <v>1260</v>
       </c>
       <c r="G17" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H17" t="str">
-        <v>670</v>
+        <v>10</v>
       </c>
       <c r="I17" t="str">
-        <v>1260</v>
+        <v>1</v>
       </c>
       <c r="J17" t="str">
-        <v>50</v>
+        <v>710</v>
       </c>
       <c r="K17" t="str">
-        <v>10</v>
+        <v>1305</v>
       </c>
       <c r="L17" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M17" t="str">
-        <v>710</v>
+        <v>54</v>
       </c>
       <c r="N17" t="str">
-        <v>1305</v>
-      </c>
-      <c r="O17" t="str">
-        <v>270</v>
-      </c>
-      <c r="P17" t="str">
-        <v>54</v>
-      </c>
-      <c r="Q17" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1295,42 +1142,33 @@
         <v>Aluminium Panel Heater AM-W (350W)</v>
       </c>
       <c r="E18" t="str">
-        <v>595</v>
+        <v>670</v>
       </c>
       <c r="F18" t="str">
-        <v>595</v>
+        <v>660</v>
       </c>
       <c r="G18" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H18" t="str">
-        <v>670</v>
+        <v>4.78</v>
       </c>
       <c r="I18" t="str">
-        <v>660</v>
+        <v>1</v>
       </c>
       <c r="J18" t="str">
-        <v>50</v>
+        <v>705</v>
       </c>
       <c r="K18" t="str">
-        <v>4.78</v>
+        <v>705</v>
       </c>
       <c r="L18" t="str">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="M18" t="str">
-        <v>705</v>
+        <v>25.92</v>
       </c>
       <c r="N18" t="str">
-        <v>705</v>
-      </c>
-      <c r="O18" t="str">
-        <v>250</v>
-      </c>
-      <c r="P18" t="str">
-        <v>25.92</v>
-      </c>
-      <c r="Q18" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1348,42 +1186,33 @@
         <v>Aluminium Panel Heater AM-W (500W)</v>
       </c>
       <c r="E19" t="str">
-        <v>795</v>
+        <v>670</v>
       </c>
       <c r="F19" t="str">
-        <v>595</v>
+        <v>860</v>
       </c>
       <c r="G19" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H19" t="str">
-        <v>670</v>
+        <v>6.5</v>
       </c>
       <c r="I19" t="str">
-        <v>860</v>
+        <v>1</v>
       </c>
       <c r="J19" t="str">
-        <v>50</v>
+        <v>705</v>
       </c>
       <c r="K19" t="str">
-        <v>6.5</v>
+        <v>870</v>
       </c>
       <c r="L19" t="str">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="M19" t="str">
-        <v>705</v>
+        <v>35.33</v>
       </c>
       <c r="N19" t="str">
-        <v>870</v>
-      </c>
-      <c r="O19" t="str">
-        <v>265</v>
-      </c>
-      <c r="P19" t="str">
-        <v>35.33</v>
-      </c>
-      <c r="Q19" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1401,42 +1230,33 @@
         <v>Aluminium Panel Heater AM-W (800W)</v>
       </c>
       <c r="E20" t="str">
-        <v>1195</v>
+        <v>670</v>
       </c>
       <c r="F20" t="str">
-        <v>595</v>
+        <v>1260</v>
       </c>
       <c r="G20" t="str">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H20" t="str">
-        <v>670</v>
+        <v>10</v>
       </c>
       <c r="I20" t="str">
-        <v>1260</v>
+        <v>1</v>
       </c>
       <c r="J20" t="str">
-        <v>50</v>
+        <v>710</v>
       </c>
       <c r="K20" t="str">
-        <v>10</v>
+        <v>1305</v>
       </c>
       <c r="L20" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M20" t="str">
-        <v>710</v>
+        <v>54</v>
       </c>
       <c r="N20" t="str">
-        <v>1305</v>
-      </c>
-      <c r="O20" t="str">
-        <v>270</v>
-      </c>
-      <c r="P20" t="str">
-        <v>54</v>
-      </c>
-      <c r="Q20" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1454,42 +1274,33 @@
         <v>Aluminium Plinth Panel W 70W</v>
       </c>
       <c r="E21" t="str">
-        <v>500</v>
+        <v>165</v>
       </c>
       <c r="F21" t="str">
-        <v>150</v>
+        <v>560</v>
       </c>
       <c r="G21" t="str">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="H21" t="str">
-        <v>165</v>
+        <v>1.3</v>
       </c>
       <c r="I21" t="str">
-        <v>560</v>
+        <v>1</v>
       </c>
       <c r="J21" t="str">
-        <v>48</v>
+        <v>542</v>
       </c>
       <c r="K21" t="str">
-        <v>1.3</v>
+        <v>580</v>
       </c>
       <c r="L21" t="str">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="M21" t="str">
-        <v>542</v>
+        <v>21</v>
       </c>
       <c r="N21" t="str">
-        <v>580</v>
-      </c>
-      <c r="O21" t="str">
-        <v>200</v>
-      </c>
-      <c r="P21" t="str">
-        <v>21</v>
-      </c>
-      <c r="Q21" t="str">
         <v>15</v>
       </c>
     </row>
@@ -1507,42 +1318,33 @@
         <v>Mirror Heater (350W)</v>
       </c>
       <c r="E22" t="str">
-        <v>700</v>
+        <v>670</v>
       </c>
       <c r="F22" t="str">
-        <v>600</v>
+        <v>770</v>
       </c>
       <c r="G22" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H22" t="str">
-        <v>670</v>
+        <v>8.92</v>
       </c>
       <c r="I22" t="str">
-        <v>770</v>
+        <v>1</v>
       </c>
       <c r="J22" t="str">
-        <v>50</v>
+        <v>810</v>
       </c>
       <c r="K22" t="str">
-        <v>8.92</v>
+        <v>720</v>
       </c>
       <c r="L22" t="str">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="M22" t="str">
-        <v>810</v>
+        <v>47</v>
       </c>
       <c r="N22" t="str">
-        <v>720</v>
-      </c>
-      <c r="O22" t="str">
-        <v>27</v>
-      </c>
-      <c r="P22" t="str">
-        <v>47</v>
-      </c>
-      <c r="Q22" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1560,42 +1362,33 @@
         <v>Mirror Heater (500W)</v>
       </c>
       <c r="E23" t="str">
-        <v>1000</v>
+        <v>630</v>
       </c>
       <c r="F23" t="str">
-        <v>600</v>
+        <v>1160</v>
       </c>
       <c r="G23" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H23" t="str">
-        <v>630</v>
+        <v>12.4</v>
       </c>
       <c r="I23" t="str">
-        <v>1160</v>
+        <v>1</v>
       </c>
       <c r="J23" t="str">
-        <v>50</v>
+        <v>680</v>
       </c>
       <c r="K23" t="str">
-        <v>12.4</v>
+        <v>1200</v>
       </c>
       <c r="L23" t="str">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="M23" t="str">
-        <v>680</v>
+        <v>65.5</v>
       </c>
       <c r="N23" t="str">
-        <v>1200</v>
-      </c>
-      <c r="O23" t="str">
-        <v>27</v>
-      </c>
-      <c r="P23" t="str">
-        <v>65.5</v>
-      </c>
-      <c r="Q23" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1613,42 +1406,33 @@
         <v>Mirror Heater LED (350W)</v>
       </c>
       <c r="E24" t="str">
-        <v>700</v>
+        <v>770</v>
       </c>
       <c r="F24" t="str">
-        <v>600</v>
+        <v>665</v>
       </c>
       <c r="G24" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H24" t="str">
-        <v>770</v>
+        <v>9.59</v>
       </c>
       <c r="I24" t="str">
-        <v>665</v>
+        <v>1</v>
       </c>
       <c r="J24" t="str">
-        <v>50</v>
+        <v>810</v>
       </c>
       <c r="K24" t="str">
-        <v>9.59</v>
+        <v>720</v>
       </c>
       <c r="L24" t="str">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="M24" t="str">
-        <v>810</v>
+        <v>60.4</v>
       </c>
       <c r="N24" t="str">
-        <v>720</v>
-      </c>
-      <c r="O24" t="str">
-        <v>27</v>
-      </c>
-      <c r="P24" t="str">
-        <v>60.4</v>
-      </c>
-      <c r="Q24" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1666,42 +1450,33 @@
         <v>Mirror Heater LED (500W)</v>
       </c>
       <c r="E25" t="str">
-        <v>1000</v>
+        <v>630</v>
       </c>
       <c r="F25" t="str">
-        <v>600</v>
+        <v>1160</v>
       </c>
       <c r="G25" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H25" t="str">
-        <v>630</v>
+        <v>13.3</v>
       </c>
       <c r="I25" t="str">
-        <v>1160</v>
+        <v>1</v>
       </c>
       <c r="J25" t="str">
-        <v>50</v>
+        <v>680</v>
       </c>
       <c r="K25" t="str">
-        <v>13.3</v>
+        <v>1200</v>
       </c>
       <c r="L25" t="str">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="M25" t="str">
-        <v>680</v>
+        <v>70</v>
       </c>
       <c r="N25" t="str">
-        <v>1200</v>
-      </c>
-      <c r="O25" t="str">
-        <v>27</v>
-      </c>
-      <c r="P25" t="str">
-        <v>70</v>
-      </c>
-      <c r="Q25" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1719,42 +1494,33 @@
         <v>Mirror Heater Round (500W)</v>
       </c>
       <c r="E26" t="str">
-        <v>32</v>
+        <v>920</v>
       </c>
       <c r="F26" t="str">
-        <v>980</v>
+        <v>930</v>
       </c>
       <c r="G26" t="str">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="H26" t="str">
+        <v>13.83</v>
+      </c>
+      <c r="I26" t="str">
+        <v>1</v>
+      </c>
+      <c r="J26" t="str">
         <v>920</v>
       </c>
-      <c r="I26" t="str">
+      <c r="K26" t="str">
         <v>930</v>
       </c>
-      <c r="J26" t="str">
+      <c r="L26" t="str">
         <v>55</v>
       </c>
-      <c r="K26" t="str">
+      <c r="M26" t="str">
         <v>13.83</v>
       </c>
-      <c r="L26" t="str">
-        <v>1</v>
-      </c>
-      <c r="M26" t="str">
-        <v>920</v>
-      </c>
       <c r="N26" t="str">
-        <v>930</v>
-      </c>
-      <c r="O26" t="str">
-        <v>55</v>
-      </c>
-      <c r="P26" t="str">
-        <v>13.83</v>
-      </c>
-      <c r="Q26" t="str">
         <v>1</v>
       </c>
     </row>
@@ -1772,42 +1538,33 @@
         <v>Mirror Heater Round LED (500W)</v>
       </c>
       <c r="E27" t="str">
-        <v>32</v>
+        <v>920</v>
       </c>
       <c r="F27" t="str">
-        <v>980</v>
+        <v>930</v>
       </c>
       <c r="G27" t="str">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="H27" t="str">
+        <v>14.41</v>
+      </c>
+      <c r="I27" t="str">
+        <v>1</v>
+      </c>
+      <c r="J27" t="str">
         <v>920</v>
       </c>
-      <c r="I27" t="str">
+      <c r="K27" t="str">
         <v>930</v>
       </c>
-      <c r="J27" t="str">
+      <c r="L27" t="str">
         <v>55</v>
       </c>
-      <c r="K27" t="str">
+      <c r="M27" t="str">
         <v>14.41</v>
       </c>
-      <c r="L27" t="str">
-        <v>1</v>
-      </c>
-      <c r="M27" t="str">
-        <v>920</v>
-      </c>
       <c r="N27" t="str">
-        <v>930</v>
-      </c>
-      <c r="O27" t="str">
-        <v>55</v>
-      </c>
-      <c r="P27" t="str">
-        <v>14.41</v>
-      </c>
-      <c r="Q27" t="str">
         <v>1</v>
       </c>
     </row>
@@ -1825,42 +1582,33 @@
         <v>Mirror Heater Half Glass (350W)</v>
       </c>
       <c r="E28" t="str">
-        <v>1000</v>
+        <v>620</v>
       </c>
       <c r="F28" t="str">
-        <v>600</v>
+        <v>1160</v>
       </c>
       <c r="G28" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H28" t="str">
-        <v>620</v>
+        <v>11.33</v>
       </c>
       <c r="I28" t="str">
-        <v>1160</v>
+        <v>1</v>
       </c>
       <c r="J28" t="str">
-        <v>50</v>
+        <v>685</v>
       </c>
       <c r="K28" t="str">
-        <v>11.33</v>
+        <v>1210</v>
       </c>
       <c r="L28" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M28" t="str">
-        <v>685</v>
+        <v>60.15</v>
       </c>
       <c r="N28" t="str">
-        <v>1210</v>
-      </c>
-      <c r="O28" t="str">
-        <v>270</v>
-      </c>
-      <c r="P28" t="str">
-        <v>60.15</v>
-      </c>
-      <c r="Q28" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1878,42 +1626,33 @@
         <v>Mirror Heater Half Glass LED (350W)</v>
       </c>
       <c r="E29" t="str">
-        <v>1000</v>
+        <v>620</v>
       </c>
       <c r="F29" t="str">
-        <v>600</v>
+        <v>1160</v>
       </c>
       <c r="G29" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H29" t="str">
-        <v>620</v>
+        <v>11.9</v>
       </c>
       <c r="I29" t="str">
-        <v>1160</v>
+        <v>1</v>
       </c>
       <c r="J29" t="str">
-        <v>50</v>
+        <v>685</v>
       </c>
       <c r="K29" t="str">
-        <v>11.9</v>
+        <v>1210</v>
       </c>
       <c r="L29" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M29" t="str">
-        <v>685</v>
+        <v>63</v>
       </c>
       <c r="N29" t="str">
-        <v>1210</v>
-      </c>
-      <c r="O29" t="str">
-        <v>270</v>
-      </c>
-      <c r="P29" t="str">
-        <v>63</v>
-      </c>
-      <c r="Q29" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1931,42 +1670,33 @@
         <v>Glass Heater W (450W)</v>
       </c>
       <c r="E30" t="str">
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="F30" t="str">
-        <v>500</v>
+        <v>660</v>
       </c>
       <c r="G30" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H30" t="str">
-        <v>620</v>
+        <v>7.28</v>
       </c>
       <c r="I30" t="str">
+        <v>1</v>
+      </c>
+      <c r="J30" t="str">
         <v>660</v>
       </c>
-      <c r="J30" t="str">
-        <v>50</v>
-      </c>
       <c r="K30" t="str">
-        <v>7.28</v>
+        <v>690</v>
       </c>
       <c r="L30" t="str">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="M30" t="str">
-        <v>660</v>
+        <v>36.88</v>
       </c>
       <c r="N30" t="str">
-        <v>690</v>
-      </c>
-      <c r="O30" t="str">
-        <v>250</v>
-      </c>
-      <c r="P30" t="str">
-        <v>36.88</v>
-      </c>
-      <c r="Q30" t="str">
         <v>5</v>
       </c>
     </row>
@@ -1984,42 +1714,33 @@
         <v>Glass Heater W (900W)</v>
       </c>
       <c r="E31" t="str">
-        <v>1100</v>
+        <v>625</v>
       </c>
       <c r="F31" t="str">
-        <v>550</v>
+        <v>1165</v>
       </c>
       <c r="G31" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H31" t="str">
-        <v>625</v>
+        <v>13.83</v>
       </c>
       <c r="I31" t="str">
-        <v>1165</v>
+        <v>1</v>
       </c>
       <c r="J31" t="str">
-        <v>50</v>
+        <v>680</v>
       </c>
       <c r="K31" t="str">
-        <v>13.83</v>
+        <v>1200</v>
       </c>
       <c r="L31" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M31" t="str">
-        <v>680</v>
+        <v>71.15</v>
       </c>
       <c r="N31" t="str">
-        <v>1200</v>
-      </c>
-      <c r="O31" t="str">
-        <v>270</v>
-      </c>
-      <c r="P31" t="str">
-        <v>71.15</v>
-      </c>
-      <c r="Q31" t="str">
         <v>5</v>
       </c>
     </row>
@@ -2037,42 +1758,33 @@
         <v>Glass Heater B (900W)</v>
       </c>
       <c r="E32" t="str">
-        <v>1100</v>
+        <v>625</v>
       </c>
       <c r="F32" t="str">
-        <v>550</v>
+        <v>1165</v>
       </c>
       <c r="G32" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H32" t="str">
-        <v>625</v>
+        <v>13.83</v>
       </c>
       <c r="I32" t="str">
-        <v>1165</v>
+        <v>1</v>
       </c>
       <c r="J32" t="str">
-        <v>50</v>
+        <v>680</v>
       </c>
       <c r="K32" t="str">
-        <v>13.83</v>
+        <v>1200</v>
       </c>
       <c r="L32" t="str">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="M32" t="str">
-        <v>680</v>
+        <v>71.15</v>
       </c>
       <c r="N32" t="str">
-        <v>1200</v>
-      </c>
-      <c r="O32" t="str">
-        <v>270</v>
-      </c>
-      <c r="P32" t="str">
-        <v>71.15</v>
-      </c>
-      <c r="Q32" t="str">
         <v>5</v>
       </c>
     </row>
@@ -2090,42 +1802,33 @@
         <v>Glass Heater B (600W)</v>
       </c>
       <c r="E33" t="str">
-        <v>1800</v>
+        <v>375</v>
       </c>
       <c r="F33" t="str">
-        <v>300</v>
+        <v>1835</v>
       </c>
       <c r="G33" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H33" t="str">
-        <v>375</v>
+        <v>11.56</v>
       </c>
       <c r="I33" t="str">
-        <v>1835</v>
+        <v>1</v>
       </c>
       <c r="J33" t="str">
-        <v>50</v>
+        <v>415</v>
       </c>
       <c r="K33" t="str">
-        <v>11.56</v>
+        <v>1865</v>
       </c>
       <c r="L33" t="str">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="M33" t="str">
-        <v>415</v>
+        <v>23.35</v>
       </c>
       <c r="N33" t="str">
-        <v>1865</v>
-      </c>
-      <c r="O33" t="str">
-        <v>110</v>
-      </c>
-      <c r="P33" t="str">
-        <v>23.35</v>
-      </c>
-      <c r="Q33" t="str">
         <v>2</v>
       </c>
     </row>
@@ -2143,42 +1846,33 @@
         <v>Glass Heater W (600W)</v>
       </c>
       <c r="E34" t="str">
-        <v>1800</v>
+        <v>375</v>
       </c>
       <c r="F34" t="str">
-        <v>300</v>
+        <v>1835</v>
       </c>
       <c r="G34" t="str">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="H34" t="str">
-        <v>375</v>
+        <v>11.56</v>
       </c>
       <c r="I34" t="str">
-        <v>1835</v>
+        <v>1</v>
       </c>
       <c r="J34" t="str">
-        <v>50</v>
+        <v>415</v>
       </c>
       <c r="K34" t="str">
-        <v>11.56</v>
+        <v>1865</v>
       </c>
       <c r="L34" t="str">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="M34" t="str">
-        <v>415</v>
+        <v>23.35</v>
       </c>
       <c r="N34" t="str">
-        <v>1865</v>
-      </c>
-      <c r="O34" t="str">
-        <v>110</v>
-      </c>
-      <c r="P34" t="str">
-        <v>23.35</v>
-      </c>
-      <c r="Q34" t="str">
         <v>2</v>
       </c>
     </row>
@@ -2196,42 +1890,33 @@
         <v>Aluminium Curved Panel Heater R (400W)</v>
       </c>
       <c r="E35" t="str">
-        <v>500</v>
+        <v>545</v>
       </c>
       <c r="F35" t="str">
-        <v>550</v>
+        <v>580</v>
       </c>
       <c r="G35" t="str">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="H35" t="str">
+        <v>3</v>
+      </c>
+      <c r="I35" t="str">
+        <v>1</v>
+      </c>
+      <c r="J35" t="str">
         <v>545</v>
       </c>
-      <c r="I35" t="str">
+      <c r="K35" t="str">
         <v>580</v>
       </c>
-      <c r="J35" t="str">
+      <c r="L35" t="str">
         <v>200</v>
       </c>
-      <c r="K35" t="str">
+      <c r="M35" t="str">
         <v>3</v>
       </c>
-      <c r="L35" t="str">
-        <v>1</v>
-      </c>
-      <c r="M35" t="str">
-        <v>545</v>
-      </c>
       <c r="N35" t="str">
-        <v>580</v>
-      </c>
-      <c r="O35" t="str">
-        <v>200</v>
-      </c>
-      <c r="P35" t="str">
-        <v>3</v>
-      </c>
-      <c r="Q35" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2249,42 +1934,33 @@
         <v>Aluminium Curved Panel Heater B (400W)</v>
       </c>
       <c r="E36" t="str">
-        <v>500</v>
+        <v>545</v>
       </c>
       <c r="F36" t="str">
-        <v>550</v>
+        <v>580</v>
       </c>
       <c r="G36" t="str">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="H36" t="str">
+        <v>3</v>
+      </c>
+      <c r="I36" t="str">
+        <v>1</v>
+      </c>
+      <c r="J36" t="str">
         <v>545</v>
       </c>
-      <c r="I36" t="str">
+      <c r="K36" t="str">
         <v>580</v>
       </c>
-      <c r="J36" t="str">
+      <c r="L36" t="str">
         <v>200</v>
       </c>
-      <c r="K36" t="str">
+      <c r="M36" t="str">
         <v>3</v>
       </c>
-      <c r="L36" t="str">
-        <v>1</v>
-      </c>
-      <c r="M36" t="str">
-        <v>545</v>
-      </c>
       <c r="N36" t="str">
-        <v>580</v>
-      </c>
-      <c r="O36" t="str">
-        <v>200</v>
-      </c>
-      <c r="P36" t="str">
-        <v>3</v>
-      </c>
-      <c r="Q36" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2302,42 +1978,33 @@
         <v>Aluminium Curved Panel Heater White (400W)</v>
       </c>
       <c r="E37" t="str">
-        <v>500</v>
+        <v>545</v>
       </c>
       <c r="F37" t="str">
-        <v>550</v>
+        <v>580</v>
       </c>
       <c r="G37" t="str">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="H37" t="str">
+        <v>3</v>
+      </c>
+      <c r="I37" t="str">
+        <v>1</v>
+      </c>
+      <c r="J37" t="str">
         <v>545</v>
       </c>
-      <c r="I37" t="str">
+      <c r="K37" t="str">
         <v>580</v>
       </c>
-      <c r="J37" t="str">
+      <c r="L37" t="str">
         <v>200</v>
       </c>
-      <c r="K37" t="str">
+      <c r="M37" t="str">
         <v>3</v>
       </c>
-      <c r="L37" t="str">
-        <v>1</v>
-      </c>
-      <c r="M37" t="str">
-        <v>545</v>
-      </c>
       <c r="N37" t="str">
-        <v>580</v>
-      </c>
-      <c r="O37" t="str">
-        <v>200</v>
-      </c>
-      <c r="P37" t="str">
-        <v>3</v>
-      </c>
-      <c r="Q37" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2355,42 +2022,33 @@
         <v>Hand Dryer (1400W)</v>
       </c>
       <c r="E38" t="str">
-        <v>295</v>
+        <v>365</v>
       </c>
       <c r="F38" t="str">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="G38" t="str">
-        <v>170</v>
+        <v>216</v>
       </c>
       <c r="H38" t="str">
-        <v>365</v>
+        <v>4.6</v>
       </c>
       <c r="I38" t="str">
-        <v>328</v>
+        <v>1</v>
       </c>
       <c r="J38" t="str">
-        <v>216</v>
+        <v>370</v>
       </c>
       <c r="K38" t="str">
-        <v>4.6</v>
+        <v>660</v>
       </c>
       <c r="L38" t="str">
-        <v>1</v>
+        <v>660</v>
       </c>
       <c r="M38" t="str">
-        <v>370</v>
+        <v>26.8</v>
       </c>
       <c r="N38" t="str">
-        <v>660</v>
-      </c>
-      <c r="O38" t="str">
-        <v>660</v>
-      </c>
-      <c r="P38" t="str">
-        <v>26.8</v>
-      </c>
-      <c r="Q38" t="str">
         <v>4</v>
       </c>
     </row>
@@ -2408,42 +2066,33 @@
         <v>High Output Heater (1000W)</v>
       </c>
       <c r="E39" t="str">
-        <v>189</v>
+        <v>137</v>
       </c>
       <c r="F39" t="str">
-        <v>600</v>
+        <v>1115</v>
       </c>
       <c r="G39" t="str">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="H39" t="str">
+        <v>4.8</v>
+      </c>
+      <c r="I39" t="str">
+        <v>1</v>
+      </c>
+      <c r="J39" t="str">
         <v>137</v>
       </c>
-      <c r="I39" t="str">
+      <c r="K39" t="str">
         <v>1115</v>
       </c>
-      <c r="J39" t="str">
+      <c r="L39" t="str">
         <v>188</v>
       </c>
-      <c r="K39" t="str">
-        <v>4.8</v>
-      </c>
-      <c r="L39" t="str">
-        <v>1</v>
-      </c>
       <c r="M39" t="str">
-        <v>137</v>
+        <v>5.6</v>
       </c>
       <c r="N39" t="str">
-        <v>1115</v>
-      </c>
-      <c r="O39" t="str">
-        <v>188</v>
-      </c>
-      <c r="P39" t="str">
-        <v>5.6</v>
-      </c>
-      <c r="Q39" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2461,42 +2110,33 @@
         <v>High Output Heater (1800W)</v>
       </c>
       <c r="E40" t="str">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="F40" t="str">
-        <v>1000</v>
+        <v>1110</v>
       </c>
       <c r="G40" t="str">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="H40" t="str">
+        <v>5.4</v>
+      </c>
+      <c r="I40" t="str">
+        <v>1</v>
+      </c>
+      <c r="J40" t="str">
         <v>200</v>
       </c>
-      <c r="I40" t="str">
+      <c r="K40" t="str">
         <v>1110</v>
       </c>
-      <c r="J40" t="str">
+      <c r="L40" t="str">
         <v>138</v>
       </c>
-      <c r="K40" t="str">
-        <v>5.4</v>
-      </c>
-      <c r="L40" t="str">
-        <v>1</v>
-      </c>
       <c r="M40" t="str">
-        <v>200</v>
+        <v>6.3</v>
       </c>
       <c r="N40" t="str">
-        <v>1110</v>
-      </c>
-      <c r="O40" t="str">
-        <v>138</v>
-      </c>
-      <c r="P40" t="str">
-        <v>6.3</v>
-      </c>
-      <c r="Q40" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2514,42 +2154,33 @@
         <v>High Output Heater (2400W)</v>
       </c>
       <c r="E41" t="str">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="F41" t="str">
-        <v>1500</v>
+        <v>1570</v>
       </c>
       <c r="G41" t="str">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="H41" t="str">
+        <v>6.5</v>
+      </c>
+      <c r="I41" t="str">
+        <v>1</v>
+      </c>
+      <c r="J41" t="str">
         <v>136</v>
       </c>
-      <c r="I41" t="str">
+      <c r="K41" t="str">
         <v>1570</v>
       </c>
-      <c r="J41" t="str">
+      <c r="L41" t="str">
         <v>190</v>
       </c>
-      <c r="K41" t="str">
-        <v>6.5</v>
-      </c>
-      <c r="L41" t="str">
-        <v>1</v>
-      </c>
       <c r="M41" t="str">
-        <v>136</v>
+        <v>7.4</v>
       </c>
       <c r="N41" t="str">
-        <v>1570</v>
-      </c>
-      <c r="O41" t="str">
-        <v>190</v>
-      </c>
-      <c r="P41" t="str">
-        <v>7.4</v>
-      </c>
-      <c r="Q41" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2567,42 +2198,33 @@
         <v>High Output Heater (3200W)</v>
       </c>
       <c r="E42" t="str">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="F42" t="str">
-        <v>2000</v>
+        <v>1980</v>
       </c>
       <c r="G42" t="str">
-        <v>67</v>
+        <v>195</v>
       </c>
       <c r="H42" t="str">
+        <v>8.2</v>
+      </c>
+      <c r="I42" t="str">
+        <v>1</v>
+      </c>
+      <c r="J42" t="str">
         <v>140</v>
       </c>
-      <c r="I42" t="str">
+      <c r="K42" t="str">
         <v>1980</v>
       </c>
-      <c r="J42" t="str">
+      <c r="L42" t="str">
         <v>195</v>
       </c>
-      <c r="K42" t="str">
-        <v>8.2</v>
-      </c>
-      <c r="L42" t="str">
-        <v>1</v>
-      </c>
       <c r="M42" t="str">
-        <v>140</v>
+        <v>10.68</v>
       </c>
       <c r="N42" t="str">
-        <v>1980</v>
-      </c>
-      <c r="O42" t="str">
-        <v>195</v>
-      </c>
-      <c r="P42" t="str">
-        <v>10.68</v>
-      </c>
-      <c r="Q42" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2620,42 +2242,33 @@
         <v>Thermostat for High Output Heater</v>
       </c>
       <c r="E43" t="str">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="F43" t="str">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="G43" t="str">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="H43" t="str">
-        <v>100</v>
+        <v>0.2</v>
       </c>
       <c r="I43" t="str">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="J43" t="str">
-        <v>65</v>
+        <v>550</v>
       </c>
       <c r="K43" t="str">
-        <v>0.2</v>
+        <v>580</v>
       </c>
       <c r="L43" t="str">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="M43" t="str">
-        <v>550</v>
+        <v>11.2</v>
       </c>
       <c r="N43" t="str">
-        <v>580</v>
-      </c>
-      <c r="O43" t="str">
-        <v>205</v>
-      </c>
-      <c r="P43" t="str">
-        <v>11.2</v>
-      </c>
-      <c r="Q43" t="str">
         <v>50</v>
       </c>
     </row>
@@ -2673,42 +2286,33 @@
         <v>Blade Bar Heater with Remote (1800W)</v>
       </c>
       <c r="E44" t="str">
+        <v>200</v>
+      </c>
+      <c r="F44" t="str">
+        <v>780</v>
+      </c>
+      <c r="G44" t="str">
+        <v>160</v>
+      </c>
+      <c r="H44" t="str">
+        <v>3.57</v>
+      </c>
+      <c r="I44" t="str">
+        <v>1</v>
+      </c>
+      <c r="J44" t="str">
+        <v>610</v>
+      </c>
+      <c r="K44" t="str">
+        <v>795</v>
+      </c>
+      <c r="L44" t="str">
         <v>170</v>
       </c>
-      <c r="F44" t="str">
-        <v>902</v>
-      </c>
-      <c r="G44" t="str">
-        <v>78</v>
-      </c>
-      <c r="H44" t="str">
-        <v>200</v>
-      </c>
-      <c r="I44" t="str">
-        <v>780</v>
-      </c>
-      <c r="J44" t="str">
-        <v>160</v>
-      </c>
-      <c r="K44" t="str">
-        <v>3.57</v>
-      </c>
-      <c r="L44" t="str">
-        <v>1</v>
-      </c>
       <c r="M44" t="str">
-        <v>610</v>
+        <v>11.83</v>
       </c>
       <c r="N44" t="str">
-        <v>795</v>
-      </c>
-      <c r="O44" t="str">
-        <v>170</v>
-      </c>
-      <c r="P44" t="str">
-        <v>11.83</v>
-      </c>
-      <c r="Q44" t="str">
         <v>3</v>
       </c>
     </row>
@@ -2726,42 +2330,33 @@
         <v>Blade Bar Heater lamp</v>
       </c>
       <c r="E45" t="str">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="F45" t="str">
         <v>600</v>
       </c>
       <c r="G45" t="str">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="H45" t="str">
-        <v>70</v>
+        <v>0.41</v>
       </c>
       <c r="I45" t="str">
-        <v>600</v>
+        <v>5</v>
       </c>
       <c r="J45" t="str">
         <v>70</v>
       </c>
       <c r="K45" t="str">
+        <v>620</v>
+      </c>
+      <c r="L45" t="str">
+        <v>70</v>
+      </c>
+      <c r="M45" t="str">
         <v>0.41</v>
       </c>
-      <c r="L45" t="str">
-        <v>5</v>
-      </c>
-      <c r="M45" t="str">
-        <v>70</v>
-      </c>
       <c r="N45" t="str">
-        <v>620</v>
-      </c>
-      <c r="O45" t="str">
-        <v>70</v>
-      </c>
-      <c r="P45" t="str">
-        <v>0.41</v>
-      </c>
-      <c r="Q45" t="str">
         <v>5</v>
       </c>
     </row>
@@ -2779,42 +2374,33 @@
         <v>Blade Bar Heater Stand 2.4m</v>
       </c>
       <c r="E46" t="str">
-        <v>0</v>
+        <v>430</v>
       </c>
       <c r="F46" t="str">
-        <v>0</v>
+        <v>630</v>
       </c>
       <c r="G46" t="str">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="H46" t="str">
+        <v>24</v>
+      </c>
+      <c r="I46" t="str">
+        <v>1</v>
+      </c>
+      <c r="J46" t="str">
         <v>430</v>
       </c>
-      <c r="I46" t="str">
+      <c r="K46" t="str">
         <v>630</v>
       </c>
-      <c r="J46" t="str">
+      <c r="L46" t="str">
         <v>205</v>
       </c>
-      <c r="K46" t="str">
+      <c r="M46" t="str">
         <v>24</v>
       </c>
-      <c r="L46" t="str">
-        <v>1</v>
-      </c>
-      <c r="M46" t="str">
-        <v>430</v>
-      </c>
       <c r="N46" t="str">
-        <v>630</v>
-      </c>
-      <c r="O46" t="str">
-        <v>205</v>
-      </c>
-      <c r="P46" t="str">
-        <v>24</v>
-      </c>
-      <c r="Q46" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2832,42 +2418,33 @@
         <v>Ceramic Glass Infrared Panel (1500W)</v>
       </c>
       <c r="E47" t="str">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="F47" t="str">
-        <v>902</v>
+        <v>1020</v>
       </c>
       <c r="G47" t="str">
-        <v>78</v>
+        <v>245</v>
       </c>
       <c r="H47" t="str">
+        <v>6.41</v>
+      </c>
+      <c r="I47" t="str">
+        <v>1</v>
+      </c>
+      <c r="J47" t="str">
         <v>190</v>
       </c>
-      <c r="I47" t="str">
+      <c r="K47" t="str">
         <v>1020</v>
       </c>
-      <c r="J47" t="str">
+      <c r="L47" t="str">
         <v>245</v>
       </c>
-      <c r="K47" t="str">
-        <v>6.41</v>
-      </c>
-      <c r="L47" t="str">
-        <v>1</v>
-      </c>
       <c r="M47" t="str">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="N47" t="str">
-        <v>1020</v>
-      </c>
-      <c r="O47" t="str">
-        <v>245</v>
-      </c>
-      <c r="P47" t="str">
-        <v>7</v>
-      </c>
-      <c r="Q47" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2885,42 +2462,33 @@
         <v>Ceramic Glass Infrared Panel (1800W)</v>
       </c>
       <c r="E48" t="str">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="F48" t="str">
-        <v>902</v>
+        <v>1020</v>
       </c>
       <c r="G48" t="str">
-        <v>78</v>
+        <v>245</v>
       </c>
       <c r="H48" t="str">
+        <v>6.41</v>
+      </c>
+      <c r="I48" t="str">
+        <v>1</v>
+      </c>
+      <c r="J48" t="str">
         <v>190</v>
       </c>
-      <c r="I48" t="str">
+      <c r="K48" t="str">
         <v>1020</v>
       </c>
-      <c r="J48" t="str">
+      <c r="L48" t="str">
         <v>245</v>
       </c>
-      <c r="K48" t="str">
-        <v>6.41</v>
-      </c>
-      <c r="L48" t="str">
-        <v>1</v>
-      </c>
       <c r="M48" t="str">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="N48" t="str">
-        <v>1020</v>
-      </c>
-      <c r="O48" t="str">
-        <v>245</v>
-      </c>
-      <c r="P48" t="str">
-        <v>7</v>
-      </c>
-      <c r="Q48" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2938,42 +2506,33 @@
         <v>Ceramic Glass Infrared Panel (2200W)</v>
       </c>
       <c r="E49" t="str">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="F49" t="str">
-        <v>902</v>
+        <v>1020</v>
       </c>
       <c r="G49" t="str">
-        <v>78</v>
+        <v>245</v>
       </c>
       <c r="H49" t="str">
+        <v>6.41</v>
+      </c>
+      <c r="I49" t="str">
+        <v>1</v>
+      </c>
+      <c r="J49" t="str">
         <v>190</v>
       </c>
-      <c r="I49" t="str">
+      <c r="K49" t="str">
         <v>1020</v>
       </c>
-      <c r="J49" t="str">
+      <c r="L49" t="str">
         <v>245</v>
       </c>
-      <c r="K49" t="str">
-        <v>6.41</v>
-      </c>
-      <c r="L49" t="str">
-        <v>1</v>
-      </c>
       <c r="M49" t="str">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="N49" t="str">
-        <v>1020</v>
-      </c>
-      <c r="O49" t="str">
-        <v>245</v>
-      </c>
-      <c r="P49" t="str">
-        <v>7</v>
-      </c>
-      <c r="Q49" t="str">
         <v>1</v>
       </c>
     </row>
@@ -2991,42 +2550,33 @@
         <v>Ceramic Glass Infrared Panel (remote)1500W</v>
       </c>
       <c r="E50" t="str">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="F50" t="str">
-        <v>902</v>
+        <v>1020</v>
       </c>
       <c r="G50" t="str">
-        <v>78</v>
+        <v>245</v>
       </c>
       <c r="H50" t="str">
+        <v>6.41</v>
+      </c>
+      <c r="I50" t="str">
+        <v>1</v>
+      </c>
+      <c r="J50" t="str">
         <v>190</v>
       </c>
-      <c r="I50" t="str">
+      <c r="K50" t="str">
         <v>1020</v>
       </c>
-      <c r="J50" t="str">
+      <c r="L50" t="str">
         <v>245</v>
       </c>
-      <c r="K50" t="str">
-        <v>6.41</v>
-      </c>
-      <c r="L50" t="str">
-        <v>1</v>
-      </c>
       <c r="M50" t="str">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="N50" t="str">
-        <v>1020</v>
-      </c>
-      <c r="O50" t="str">
-        <v>245</v>
-      </c>
-      <c r="P50" t="str">
-        <v>7</v>
-      </c>
-      <c r="Q50" t="str">
         <v>1</v>
       </c>
     </row>
@@ -3044,42 +2594,33 @@
         <v>Ceramic Glass Infrared Panel (remote)1800W</v>
       </c>
       <c r="E51" t="str">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="F51" t="str">
-        <v>902</v>
+        <v>1020</v>
       </c>
       <c r="G51" t="str">
-        <v>78</v>
+        <v>245</v>
       </c>
       <c r="H51" t="str">
+        <v>6.41</v>
+      </c>
+      <c r="I51" t="str">
+        <v>1</v>
+      </c>
+      <c r="J51" t="str">
         <v>190</v>
       </c>
-      <c r="I51" t="str">
+      <c r="K51" t="str">
         <v>1020</v>
       </c>
-      <c r="J51" t="str">
+      <c r="L51" t="str">
         <v>245</v>
       </c>
-      <c r="K51" t="str">
-        <v>6.41</v>
-      </c>
-      <c r="L51" t="str">
-        <v>1</v>
-      </c>
       <c r="M51" t="str">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="N51" t="str">
-        <v>1020</v>
-      </c>
-      <c r="O51" t="str">
-        <v>245</v>
-      </c>
-      <c r="P51" t="str">
-        <v>7</v>
-      </c>
-      <c r="Q51" t="str">
         <v>1</v>
       </c>
     </row>
@@ -3097,42 +2638,33 @@
         <v>Ceramic Glass Infrared Panel (remote) 2200W</v>
       </c>
       <c r="E52" t="str">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="F52" t="str">
-        <v>902</v>
+        <v>1020</v>
       </c>
       <c r="G52" t="str">
-        <v>78</v>
+        <v>245</v>
       </c>
       <c r="H52" t="str">
+        <v>6.41</v>
+      </c>
+      <c r="I52" t="str">
+        <v>1</v>
+      </c>
+      <c r="J52" t="str">
         <v>190</v>
       </c>
-      <c r="I52" t="str">
+      <c r="K52" t="str">
         <v>1020</v>
       </c>
-      <c r="J52" t="str">
+      <c r="L52" t="str">
         <v>245</v>
       </c>
-      <c r="K52" t="str">
-        <v>6.41</v>
-      </c>
-      <c r="L52" t="str">
-        <v>1</v>
-      </c>
       <c r="M52" t="str">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="N52" t="str">
-        <v>1020</v>
-      </c>
-      <c r="O52" t="str">
-        <v>245</v>
-      </c>
-      <c r="P52" t="str">
-        <v>7</v>
-      </c>
-      <c r="Q52" t="str">
         <v>1</v>
       </c>
     </row>
@@ -3150,42 +2682,33 @@
         <v>Heated Towel rail (120W)</v>
       </c>
       <c r="E53" t="str">
-        <v>900</v>
+        <v>530</v>
       </c>
       <c r="F53" t="str">
-        <v>500</v>
+        <v>940</v>
       </c>
       <c r="G53" t="str">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="H53" t="str">
-        <v>530</v>
+        <v>4.62</v>
       </c>
       <c r="I53" t="str">
-        <v>940</v>
+        <v>1</v>
       </c>
       <c r="J53" t="str">
-        <v>70</v>
+        <v>550</v>
       </c>
       <c r="K53" t="str">
-        <v>4.62</v>
+        <v>970</v>
       </c>
       <c r="L53" t="str">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="M53" t="str">
-        <v>550</v>
+        <v>24.57</v>
       </c>
       <c r="N53" t="str">
-        <v>970</v>
-      </c>
-      <c r="O53" t="str">
-        <v>340</v>
-      </c>
-      <c r="P53" t="str">
-        <v>24.57</v>
-      </c>
-      <c r="Q53" t="str">
         <v>5</v>
       </c>
     </row>
@@ -3203,42 +2726,33 @@
         <v>Heated Towel rail (160W)</v>
       </c>
       <c r="E54" t="str">
-        <v>900</v>
+        <v>530</v>
       </c>
       <c r="F54" t="str">
-        <v>500</v>
+        <v>940</v>
       </c>
       <c r="G54" t="str">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="H54" t="str">
-        <v>530</v>
+        <v>4.62</v>
       </c>
       <c r="I54" t="str">
-        <v>940</v>
+        <v>1</v>
       </c>
       <c r="J54" t="str">
-        <v>70</v>
+        <v>550</v>
       </c>
       <c r="K54" t="str">
-        <v>4.62</v>
+        <v>970</v>
       </c>
       <c r="L54" t="str">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="M54" t="str">
-        <v>550</v>
+        <v>24.57</v>
       </c>
       <c r="N54" t="str">
-        <v>970</v>
-      </c>
-      <c r="O54" t="str">
-        <v>340</v>
-      </c>
-      <c r="P54" t="str">
-        <v>24.57</v>
-      </c>
-      <c r="Q54" t="str">
         <v>5</v>
       </c>
     </row>
@@ -3256,42 +2770,33 @@
         <v>Heated Towel rail (320W)</v>
       </c>
       <c r="E55" t="str">
-        <v>900</v>
+        <v>530</v>
       </c>
       <c r="F55" t="str">
-        <v>500</v>
+        <v>940</v>
       </c>
       <c r="G55" t="str">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="H55" t="str">
-        <v>530</v>
+        <v>4.62</v>
       </c>
       <c r="I55" t="str">
-        <v>940</v>
+        <v>1</v>
       </c>
       <c r="J55" t="str">
-        <v>70</v>
+        <v>550</v>
       </c>
       <c r="K55" t="str">
-        <v>4.62</v>
+        <v>970</v>
       </c>
       <c r="L55" t="str">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="M55" t="str">
-        <v>550</v>
+        <v>24.57</v>
       </c>
       <c r="N55" t="str">
-        <v>970</v>
-      </c>
-      <c r="O55" t="str">
-        <v>340</v>
-      </c>
-      <c r="P55" t="str">
-        <v>24.57</v>
-      </c>
-      <c r="Q55" t="str">
         <v>5</v>
       </c>
     </row>
@@ -3309,48 +2814,39 @@
         <v>Glass Heater B (450W)</v>
       </c>
       <c r="E56" t="str">
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="F56" t="str">
-        <v>500</v>
+        <v>660</v>
       </c>
       <c r="G56" t="str">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H56" t="str">
-        <v>620</v>
+        <v>7.28</v>
       </c>
       <c r="I56" t="str">
+        <v>1</v>
+      </c>
+      <c r="J56" t="str">
         <v>660</v>
       </c>
-      <c r="J56" t="str">
-        <v>50</v>
-      </c>
       <c r="K56" t="str">
-        <v>7.28</v>
+        <v>690</v>
       </c>
       <c r="L56" t="str">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="M56" t="str">
-        <v>660</v>
+        <v>36.88</v>
       </c>
       <c r="N56" t="str">
-        <v>690</v>
-      </c>
-      <c r="O56" t="str">
-        <v>250</v>
-      </c>
-      <c r="P56" t="str">
-        <v>36.88</v>
-      </c>
-      <c r="Q56" t="str">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q56"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N56"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>